<commit_message>
Added the first 4 test cases for negative scenarious
</commit_message>
<xml_diff>
--- a/test_back/test_forms/negative_validations_scenarious_shapes/TestCases lego_assambly_backend.xlsx
+++ b/test_back/test_forms/negative_validations_scenarious_shapes/TestCases lego_assambly_backend.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Preconditions</t>
   </si>
@@ -94,15 +94,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Verify "array_cubes_empty" JSON file</t>
-  </si>
-  <si>
     <t>NEGATIVE</t>
   </si>
   <si>
-    <t>An error will be displayed</t>
-  </si>
-  <si>
     <t>Apuscasitei Silviu</t>
   </si>
   <si>
@@ -179,6 +173,198 @@
     </r>
   </si>
   <si>
+    <t>An error message will be displayed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify "array_cubes_empty" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify "color_field_missing" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>backend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> validation for "color" field missing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. to have the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>python</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>application</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                            2. to have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with that specifications</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">1. </t>
     </r>
@@ -348,7 +534,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> the command: python main.py THE_NAME_OF_JSON_FILE                    5. </t>
+      <t xml:space="preserve"> the command: python main.py array_cubes_empty                                5. </t>
     </r>
     <r>
       <rPr>
@@ -437,6 +623,654 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>download</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>github</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the application (from master)                      2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>copy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> you want to test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in the root of project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (where </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>main.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file exist)                                                     3. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>open</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cmd in the application              4. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>write</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the command: python main.py color_field_missing                                 5. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>press</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ENTER                                          6. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from project</t>
+    </r>
+  </si>
+  <si>
+    <t>TEST PASSED</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify "color_its_not_in_hexa_code_format" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>backend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> validation for hexa_code format for "color" field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>download</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>github</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the application (from master)                      2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>copy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> you want to test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in the root of project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (where </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>main.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file exist)                                                     3. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>open</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cmd in the application              4. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>write</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the command: python main.py color_its_not_in_hexa_code_format                      5. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>press</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ENTER                                          6. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from project</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It's more like a worning   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>x=0 y=0 z=0 blue 0
+A cube's color field is not in HEX"</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -455,7 +1289,430 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">                  "Please provide at least 1 cube"</t>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Oops, a cube doesn't have the color field. Each cube must have it"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEST PASSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Please provide at least 1 cube"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify "cube_with_coordinate_000_is_missing" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>backend</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> validation for missing origin cube from array</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>download</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>github</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the application (from master)                      2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>copy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> you want to test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in the root of project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (where </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>main.py</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file exist)                                                     3. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>open</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cmd in the application              4. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>write</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the command: python main.py cube_with_coordinate_000_is_missing                                                                     5. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>press</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ENTER                                          6. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JSON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from project</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>It's more like a worning</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"x=2 y=0 z=0 #FFFFFF 0
+x=1 y=0 z=0 #FFFFFF 1
+No cube with x=0, y=0, z=0 has been found"</t>
     </r>
   </si>
 </sst>
@@ -463,7 +1720,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +1757,44 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -546,7 +1841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,9 +1862,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -580,6 +1872,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -869,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,7 +2184,7 @@
     <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="19.88671875" customWidth="1"/>
     <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -896,11 +2197,11 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -924,7 +2225,7 @@
       <c r="H7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -933,59 +2234,110 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>23</v>
-      </c>
       <c r="D8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>24</v>
-      </c>
       <c r="H8" s="7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>2</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>4</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="9"/>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
@@ -993,7 +2345,7 @@
       <c r="D12" s="7"/>
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>